<commit_message>
Full functional have some bugs
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -8,16 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\SISP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49608222-DA6B-44FA-BFC5-C61B9546B458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70908A3A-59BB-4045-9D91-27DF99E5F90F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Example1" r:id="rId6" sheetId="9"/>
-    <sheet name="Example2" r:id="rId7" sheetId="10"/>
-    <sheet name="Example3" r:id="rId8" sheetId="11"/>
+    <sheet name="Лист1" sheetId="5" r:id="rId1"/>
+    <sheet name="Матрица распределения объемов к" sheetId="7" r:id="rId3"/>
+    <sheet name="Матрица интенсивностей на часов" sheetId="8" r:id="rId4"/>
+    <sheet name="Матрица привлекательности" r:id="rId8" sheetId="9"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -371,9 +383,49 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02CEB268-472F-4A46-8615-38A0738FEFED}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:N14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:N14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -384,123 +436,83 @@
         <v>0.0</v>
       </c>
       <c r="B1" t="n" s="0">
-        <v>101.7</v>
+        <v>0.171</v>
       </c>
       <c r="C1" t="n" s="0">
-        <v>127.871</v>
+        <v>0.253</v>
+      </c>
+      <c r="D1" t="n" s="0">
+        <v>0.332</v>
+      </c>
+      <c r="E1" t="n" s="0">
+        <v>0.244</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n" s="0">
-        <v>114.9216</v>
+        <v>0.121</v>
       </c>
       <c r="B2" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="C2" t="n" s="0">
-        <v>194.0074</v>
+        <v>0.268</v>
+      </c>
+      <c r="D2" t="n" s="0">
+        <v>0.352</v>
+      </c>
+      <c r="E2" t="n" s="0">
+        <v>0.259</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n" s="0">
-        <v>165.4098</v>
+        <v>0.133</v>
       </c>
       <c r="B3" t="n" s="0">
-        <v>222.8762</v>
+        <v>0.199</v>
       </c>
       <c r="C3" t="n" s="0">
         <v>0.0</v>
       </c>
+      <c r="D3" t="n" s="0">
+        <v>0.385</v>
+      </c>
+      <c r="E3" t="n" s="0">
+        <v>0.283</v>
+      </c>
     </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="n" s="0">
+    <row r="4">
+      <c r="A4" t="n" s="0">
+        <v>0.146</v>
+      </c>
+      <c r="B4" t="n" s="0">
+        <v>0.219</v>
+      </c>
+      <c r="C4" t="n" s="0">
+        <v>0.323</v>
+      </c>
+      <c r="D4" t="n" s="0">
         <v>0.0</v>
       </c>
-      <c r="B1" t="n" s="0">
-        <v>5.0E-4</v>
-      </c>
-      <c r="C1" t="n" s="0">
-        <v>6.0E-4</v>
+      <c r="E4" t="n" s="0">
+        <v>0.312</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n" s="0">
-        <v>5.0E-4</v>
-      </c>
-      <c r="B2" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="C2" t="n" s="0">
-        <v>9.0E-4</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n" s="0">
-        <v>7.0E-4</v>
-      </c>
-      <c r="B3" t="n" s="0">
-        <v>0.001</v>
-      </c>
-      <c r="C3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="B1" t="n" s="0">
-        <v>0.443</v>
-      </c>
-      <c r="C1" t="n" s="0">
-        <v>0.557</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n" s="0">
-        <v>0.372</v>
-      </c>
-      <c r="B2" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="C2" t="n" s="0">
-        <v>0.628</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n" s="0">
-        <v>0.426</v>
-      </c>
-      <c r="B3" t="n" s="0">
-        <v>0.574</v>
-      </c>
-      <c r="C3" t="n" s="0">
+    <row r="5">
+      <c r="A5" t="n" s="0">
+        <v>0.131</v>
+      </c>
+      <c r="B5" t="n" s="0">
+        <v>0.197</v>
+      </c>
+      <c r="C5" t="n" s="0">
+        <v>0.291</v>
+      </c>
+      <c r="D5" t="n" s="0">
+        <v>0.381</v>
+      </c>
+      <c r="E5" t="n" s="0">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>